<commit_message>
image loading improvements? i think???
</commit_message>
<xml_diff>
--- a/website-translations.xlsx
+++ b/website-translations.xlsx
@@ -12,6 +12,7 @@
     <sheet state="visible" name="lifestyle" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="portraits" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="brands" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="not-found" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="205">
   <si>
     <t>KEY</t>
   </si>
@@ -159,6 +160,9 @@
     <t>Read the full Testimonials</t>
   </si>
   <si>
+    <t>Read the full testimonials</t>
+  </si>
+  <si>
     <t>Lue lisää asiakaskokemuksia</t>
   </si>
   <si>
@@ -252,10 +256,19 @@
     <t>Let’s start the conversation!</t>
   </si>
   <si>
+    <t>Avataan keskustelu!</t>
+  </si>
+  <si>
     <t>Get in touch to discuss your vision</t>
   </si>
   <si>
+    <t>Ota yhteyttä ja kartoitetaan visiosi ja tarpeesi</t>
+  </si>
+  <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Nimi</t>
   </si>
   <si>
     <t>Email</t>
@@ -276,6 +289,9 @@
     <t>Feel free to add your photography needs, location, time and any special requests</t>
   </si>
   <si>
+    <t>Esimerkiksi valokuvaustarpeet, lokaatio, aikatoiveet yms.</t>
+  </si>
+  <si>
     <t>Send!</t>
   </si>
   <si>
@@ -285,7 +301,13 @@
     <t>Sending...</t>
   </si>
   <si>
+    <t>Lähetetään...</t>
+  </si>
+  <si>
     <t>Success!</t>
+  </si>
+  <si>
+    <t>Valmis!</t>
   </si>
   <si>
     <t>I'll get back</t>
@@ -294,19 +316,28 @@
     <t>I’ll get back to you at {{email}} within 48h!</t>
   </si>
   <si>
-    <t>Palaan tilaukseesi lähettämällä viestiä sähköpostiisi ({{email}})</t>
+    <t>Otan sähköpostiin ({{email}}) yhteyttä 48 tunnin kuluessa</t>
   </si>
   <si>
     <t>close</t>
   </si>
   <si>
+    <t>Sulje</t>
+  </si>
+  <si>
     <t>Error!</t>
+  </si>
+  <si>
+    <t>Virhe!</t>
   </si>
   <si>
     <t>Something went wrong</t>
   </si>
   <si>
     <t>Something went wrong, please try again later</t>
+  </si>
+  <si>
+    <t>Jokin meni pieleen, yritä myöhemmin uudelleen.</t>
   </si>
   <si>
     <t>your@email.com</t>
@@ -321,28 +352,43 @@
     <t>Some details about what you want</t>
   </si>
   <si>
+    <t>Lisää kuvaustoiveisiin liittyvä viesti</t>
+  </si>
+  <si>
     <t>ValidEmailError</t>
   </si>
   <si>
     <t>Please enter a valid email address</t>
   </si>
   <si>
+    <t>Lisää toimiva sähköpostiosoite</t>
+  </si>
+  <si>
     <t>NameMustNotBeEmptyError</t>
   </si>
   <si>
-    <t>Your name must not be empty</t>
+    <t>Must include name</t>
+  </si>
+  <si>
+    <t>Lisää nimi</t>
   </si>
   <si>
     <t>DetailsMustNotBeEmptyError</t>
   </si>
   <si>
-    <t>Your message must not be empty</t>
+    <t>Must include messge</t>
+  </si>
+  <si>
+    <t>Lisää viesti</t>
   </si>
   <si>
     <t>DetailsMustNotExceedError</t>
   </si>
   <si>
-    <t>Your message cannot exceed 2000 characters</t>
+    <t>Max. 2000 characters</t>
+  </si>
+  <si>
+    <t>Max. 2000 merkkiä</t>
   </si>
   <si>
     <t>TestimonialsIntro</t>
@@ -352,6 +398,9 @@
   </si>
   <si>
     <t>Saara</t>
+  </si>
+  <si>
+    <t>Saara, Ylioppilaskuvat</t>
   </si>
   <si>
     <t>Testimonial1</t>
@@ -444,6 +493,15 @@
     <t>Brändikuvaukset</t>
   </si>
   <si>
+    <t>BrandsExplanation</t>
+  </si>
+  <si>
+    <t>Brands, commercials, companies</t>
+  </si>
+  <si>
+    <t>Brändit, mainokset, yritykset</t>
+  </si>
+  <si>
     <t>Birthday K&amp;K</t>
   </si>
   <si>
@@ -468,19 +526,22 @@
     <t>Graduation</t>
   </si>
   <si>
-    <t>Valmistujaiset</t>
+    <t>Ylioppilasjuhlat</t>
   </si>
   <si>
     <t>Mikkeli Graduation</t>
   </si>
   <si>
-    <t>Mikkeli Road Trip (MRT)</t>
+    <t>Valmistujaiset</t>
   </si>
   <si>
-    <t>Opiskelijatapahtuma</t>
+    <t>Student Events</t>
   </si>
   <si>
-    <t>Sillis</t>
+    <t>Student events</t>
+  </si>
+  <si>
+    <t>Opiskelijatapahtumia</t>
   </si>
   <si>
     <t>Sitsit</t>
@@ -489,25 +550,64 @@
     <t>Wedding</t>
   </si>
   <si>
+    <t>Häät</t>
+  </si>
+  <si>
     <t>XXL Mössö</t>
+  </si>
+  <si>
+    <t>Festival</t>
+  </si>
+  <si>
+    <t>Festarit</t>
   </si>
   <si>
     <t>Couple B&amp;J</t>
   </si>
   <si>
+    <t>B&amp;J</t>
+  </si>
+  <si>
     <t>Engagement</t>
+  </si>
+  <si>
+    <t>Kihlajaiskuvat</t>
+  </si>
+  <si>
+    <t>Yo-kuvat</t>
   </si>
   <si>
     <t>Ondrej</t>
   </si>
   <si>
+    <t>Henkilökuvaus</t>
+  </si>
+  <si>
+    <t>Highschool graduation</t>
+  </si>
+  <si>
     <t>Beauty Salon</t>
+  </si>
+  <si>
+    <t>Kosmetologi</t>
   </si>
   <si>
     <t>FC Probba</t>
   </si>
   <si>
+    <t>Football team</t>
+  </si>
+  <si>
+    <t>Jalkapallojoukkue</t>
+  </si>
+  <si>
     <t>Riia</t>
+  </si>
+  <si>
+    <t>Personal branding</t>
+  </si>
+  <si>
+    <t>Henkilöbrändäys</t>
   </si>
   <si>
     <t>Vappu</t>
@@ -517,6 +617,24 @@
   </si>
   <si>
     <t>Yoga</t>
+  </si>
+  <si>
+    <t>Jooga</t>
+  </si>
+  <si>
+    <t>404 What are you looking for</t>
+  </si>
+  <si>
+    <t>404 | What are you looking for</t>
+  </si>
+  <si>
+    <t>404 | Mitä etsit?</t>
+  </si>
+  <si>
+    <t>Main page</t>
+  </si>
+  <si>
+    <t>Takaisin</t>
   </si>
 </sst>
 </file>
@@ -638,6 +756,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -948,6 +1070,55 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -1146,10 +1317,10 @@
         <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" s="4"/>
     </row>
@@ -5123,143 +5294,143 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E10" s="10"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>25</v>
@@ -10220,12 +10391,14 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -10252,12 +10425,14 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -10284,12 +10459,14 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -10316,13 +10493,13 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -10350,13 +10527,13 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -10384,12 +10561,14 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -10416,13 +10595,13 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -10450,12 +10629,14 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -10482,12 +10663,14 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -10514,13 +10697,13 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="9"/>
@@ -10548,12 +10731,14 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
@@ -10580,12 +10765,14 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -10612,12 +10799,14 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
@@ -10644,13 +10833,13 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -10678,12 +10867,14 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -10710,12 +10901,14 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -10742,12 +10935,14 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -10774,12 +10969,14 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -10806,12 +11003,14 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -10838,12 +11037,14 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -38329,7 +38530,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -38341,79 +38542,79 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12">
@@ -43375,6 +43576,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="19.13"/>
+    <col customWidth="1" min="3" max="3" width="24.88"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -43389,7 +43594,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -43400,72 +43605,83 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:C8">
+  <conditionalFormatting sqref="A2:C9">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
@@ -43500,97 +43716,101 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>150</v>
+        <v>169</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>153</v>
+        <v>174</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>154</v>
+        <v>175</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>156</v>
+      <c r="C10" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -43621,42 +43841,57 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>157</v>
+        <v>180</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>158</v>
+        <v>182</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>148</v>
+        <v>167</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>159</v>
+        <v>185</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>187</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -43690,54 +43925,57 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>160</v>
+        <v>188</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>162</v>
+        <v>193</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>194</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>